<commit_message>
Amazing Cybersecurity Course completed today - Total 5th in linkedin courses
</commit_message>
<xml_diff>
--- a/0_CERTIFICATES/2024-04-04_COURSE_Sheet.xlsx
+++ b/0_CERTIFICATES/2024-04-04_COURSE_Sheet.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\repos\CourseraPlus\0_CERTIFICATES\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{718E3F63-8D39-4C00-8F8D-E74540BBAF46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{184DF6D8-7474-46DC-BD6F-DE674F18FEFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="143">
   <si>
     <t>COURSERA Plus Courses</t>
   </si>
@@ -445,6 +445,30 @@
   </si>
   <si>
     <t>2024 - 01 - 08</t>
+  </si>
+  <si>
+    <t>Google Cloud Digital Cloud Leader Cert Prep: 3 Innovating with Google Cloud Artificial Intelligence</t>
+  </si>
+  <si>
+    <t>2024 - 04 - 16</t>
+  </si>
+  <si>
+    <t>2024 - 04 - 28</t>
+  </si>
+  <si>
+    <t>Advanced Machine Learning .NET Applications</t>
+  </si>
+  <si>
+    <t>2024 - 04 - 18</t>
+  </si>
+  <si>
+    <t>The Cybersecurity Threat Landscape</t>
+  </si>
+  <si>
+    <t>2024 - 04 - 24</t>
+  </si>
+  <si>
+    <t>Cybersecurity Foundations</t>
   </si>
 </sst>
 </file>
@@ -1167,7 +1191,7 @@
     </row>
     <row r="10" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B10" s="16">
-        <f t="shared" ref="B8:B70" ca="1" si="0">IFERROR(OFFSET(B10,-1,0,1,1)+1,"")</f>
+        <f t="shared" ref="B10:B70" ca="1" si="0">IFERROR(OFFSET(B10,-1,0,1,1)+1,"")</f>
         <v>6</v>
       </c>
       <c r="C10" s="17" t="s">
@@ -1303,7 +1327,7 @@
     </row>
     <row r="16" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B16" s="16">
-        <f ca="1">IFERROR(OFFSET(B16,-1,0,1,1)+1,"")</f>
+        <f t="shared" ref="B16:B40" ca="1" si="1">IFERROR(OFFSET(B16,-1,0,1,1)+1,"")</f>
         <v>12</v>
       </c>
       <c r="C16" s="17" t="s">
@@ -1326,7 +1350,7 @@
     </row>
     <row r="17" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B17" s="16">
-        <f ca="1">IFERROR(OFFSET(B17,-1,0,1,1)+1,"")</f>
+        <f t="shared" ca="1" si="1"/>
         <v>13</v>
       </c>
       <c r="C17" s="17" t="s">
@@ -1349,7 +1373,7 @@
     </row>
     <row r="18" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B18" s="16">
-        <f ca="1">IFERROR(OFFSET(B18,-1,0,1,1)+1,"")</f>
+        <f t="shared" ca="1" si="1"/>
         <v>14</v>
       </c>
       <c r="C18" s="17" t="s">
@@ -1372,7 +1396,7 @@
     </row>
     <row r="19" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B19" s="16">
-        <f ca="1">IFERROR(OFFSET(B19,-1,0,1,1)+1,"")</f>
+        <f t="shared" ca="1" si="1"/>
         <v>15</v>
       </c>
       <c r="C19" s="17" t="s">
@@ -1395,7 +1419,7 @@
     </row>
     <row r="20" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B20" s="16">
-        <f ca="1">IFERROR(OFFSET(B20,-1,0,1,1)+1,"")</f>
+        <f t="shared" ca="1" si="1"/>
         <v>16</v>
       </c>
       <c r="C20" s="17" t="s">
@@ -1418,7 +1442,7 @@
     </row>
     <row r="21" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B21" s="5">
-        <f ca="1">IFERROR(OFFSET(B21,-1,0,1,1)+1,"")</f>
+        <f t="shared" ca="1" si="1"/>
         <v>17</v>
       </c>
       <c r="C21" s="6" t="s">
@@ -1437,7 +1461,7 @@
         <v>0.06</v>
       </c>
       <c r="H21" s="26" t="str">
-        <f t="shared" ref="H21:H27" si="1">IF(G21-J21=0,"",ROUND(G21-J21,2)*100&amp;"% Better")</f>
+        <f t="shared" ref="H21:H27" si="2">IF(G21-J21=0,"",ROUND(G21-J21,2)*100&amp;"% Better")</f>
         <v>5% Better</v>
       </c>
       <c r="J21" s="24">
@@ -1446,7 +1470,7 @@
     </row>
     <row r="22" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B22" s="5">
-        <f ca="1">IFERROR(OFFSET(B22,-1,0,1,1)+1,"")</f>
+        <f t="shared" ca="1" si="1"/>
         <v>18</v>
       </c>
       <c r="C22" s="6" t="s">
@@ -1465,14 +1489,14 @@
         <v>0.21</v>
       </c>
       <c r="H22" s="26" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>21% Better</v>
       </c>
       <c r="J22" s="24"/>
     </row>
     <row r="23" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B23" s="5">
-        <f ca="1">IFERROR(OFFSET(B23,-1,0,1,1)+1,"")</f>
+        <f t="shared" ca="1" si="1"/>
         <v>19</v>
       </c>
       <c r="C23" s="6" t="s">
@@ -1491,14 +1515,14 @@
         <v>0.17</v>
       </c>
       <c r="H23" s="26" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>17% Better</v>
       </c>
       <c r="J23" s="24"/>
     </row>
     <row r="24" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B24" s="5">
-        <f ca="1">IFERROR(OFFSET(B24,-1,0,1,1)+1,"")</f>
+        <f t="shared" ca="1" si="1"/>
         <v>20</v>
       </c>
       <c r="C24" s="6" t="s">
@@ -1517,14 +1541,14 @@
         <v>0.17</v>
       </c>
       <c r="H24" s="26" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>17% Better</v>
       </c>
       <c r="J24" s="24"/>
     </row>
     <row r="25" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B25" s="5">
-        <f ca="1">IFERROR(OFFSET(B25,-1,0,1,1)+1,"")</f>
+        <f t="shared" ca="1" si="1"/>
         <v>21</v>
       </c>
       <c r="C25" s="6" t="s">
@@ -1543,13 +1567,13 @@
         <v>0.38</v>
       </c>
       <c r="H25" s="26" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>38% Better</v>
       </c>
     </row>
     <row r="26" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B26" s="5">
-        <f ca="1">IFERROR(OFFSET(B26,-1,0,1,1)+1,"")</f>
+        <f t="shared" ca="1" si="1"/>
         <v>22</v>
       </c>
       <c r="C26" s="6" t="s">
@@ -1568,7 +1592,7 @@
         <v>0.53</v>
       </c>
       <c r="H26" s="26" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>5% Better</v>
       </c>
       <c r="J26" s="24">
@@ -1577,7 +1601,7 @@
     </row>
     <row r="27" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B27" s="5">
-        <f ca="1">IFERROR(OFFSET(B27,-1,0,1,1)+1,"")</f>
+        <f t="shared" ca="1" si="1"/>
         <v>23</v>
       </c>
       <c r="C27" s="6" t="s">
@@ -1596,14 +1620,14 @@
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="H27" s="26" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>7% Better</v>
       </c>
       <c r="J27" s="24"/>
     </row>
     <row r="28" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B28" s="5">
-        <f ca="1">IFERROR(OFFSET(B28,-1,0,1,1)+1,"")</f>
+        <f t="shared" ca="1" si="1"/>
         <v>24</v>
       </c>
       <c r="C28" s="6" t="s">
@@ -1631,7 +1655,7 @@
     </row>
     <row r="29" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B29" s="5">
-        <f ca="1">IFERROR(OFFSET(B29,-1,0,1,1)+1,"")</f>
+        <f t="shared" ca="1" si="1"/>
         <v>25</v>
       </c>
       <c r="C29" s="6" t="s">
@@ -1650,7 +1674,7 @@
         <v>0.64</v>
       </c>
       <c r="H29" s="26" t="str">
-        <f t="shared" ref="H29:H32" si="2">IF(G29-J29=0,"",ROUND(G29-J29,2)*100&amp;"% Better")</f>
+        <f t="shared" ref="H29:H32" si="3">IF(G29-J29=0,"",ROUND(G29-J29,2)*100&amp;"% Better")</f>
         <v>28% Better</v>
       </c>
       <c r="J29" s="24">
@@ -1659,7 +1683,7 @@
     </row>
     <row r="30" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B30" s="5">
-        <f ca="1">IFERROR(OFFSET(B30,-1,0,1,1)+1,"")</f>
+        <f t="shared" ca="1" si="1"/>
         <v>26</v>
       </c>
       <c r="C30" s="6" t="s">
@@ -1678,14 +1702,14 @@
         <v>0.36</v>
       </c>
       <c r="H30" s="26" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>36% Better</v>
       </c>
       <c r="J30" s="24"/>
     </row>
     <row r="31" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B31" s="5">
-        <f ca="1">IFERROR(OFFSET(B31,-1,0,1,1)+1,"")</f>
+        <f t="shared" ca="1" si="1"/>
         <v>27</v>
       </c>
       <c r="C31" s="6" t="s">
@@ -1704,14 +1728,14 @@
         <v>0.2</v>
       </c>
       <c r="H31" s="26" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>20% Better</v>
       </c>
       <c r="J31" s="24"/>
     </row>
     <row r="32" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B32" s="5">
-        <f ca="1">IFERROR(OFFSET(B32,-1,0,1,1)+1,"")</f>
+        <f t="shared" ca="1" si="1"/>
         <v>28</v>
       </c>
       <c r="C32" s="6" t="s">
@@ -1730,14 +1754,14 @@
         <v>0.19</v>
       </c>
       <c r="H32" s="26" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>19% Better</v>
       </c>
       <c r="J32" s="24"/>
     </row>
     <row r="33" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B33" s="5">
-        <f ca="1">IFERROR(OFFSET(B33,-1,0,1,1)+1,"")</f>
+        <f t="shared" ca="1" si="1"/>
         <v>29</v>
       </c>
       <c r="C33" s="6" t="s">
@@ -1756,7 +1780,7 @@
         <v>0.45</v>
       </c>
       <c r="H33" s="26" t="str">
-        <f>IF(G33-J33=0,"",ROUND(G33-J33,2)*100&amp;"% Better")</f>
+        <f t="shared" ref="H33:H40" si="4">IF(G33-J33=0,"",ROUND(G33-J33,2)*100&amp;"% Better")</f>
         <v>2% Better</v>
       </c>
       <c r="J33" s="24">
@@ -1765,7 +1789,7 @@
     </row>
     <row r="34" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B34" s="5">
-        <f ca="1">IFERROR(OFFSET(B34,-1,0,1,1)+1,"")</f>
+        <f t="shared" ca="1" si="1"/>
         <v>30</v>
       </c>
       <c r="C34" s="6" t="s">
@@ -1784,7 +1808,7 @@
         <v>0.05</v>
       </c>
       <c r="H34" s="26" t="str">
-        <f>IF(G34-J34=0,"",ROUND(G34-J34,2)*100&amp;"% Better")</f>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="J34" s="24">
@@ -1793,7 +1817,7 @@
     </row>
     <row r="35" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B35" s="5">
-        <f ca="1">IFERROR(OFFSET(B35,-1,0,1,1)+1,"")</f>
+        <f t="shared" ca="1" si="1"/>
         <v>31</v>
       </c>
       <c r="C35" s="6" t="s">
@@ -1812,7 +1836,7 @@
         <v>0.26</v>
       </c>
       <c r="H35" s="26" t="str">
-        <f>IF(G35-J35=0,"",ROUND(G35-J35,2)*100&amp;"% Better")</f>
+        <f t="shared" si="4"/>
         <v>21% Better</v>
       </c>
       <c r="J35" s="24">
@@ -1821,7 +1845,7 @@
     </row>
     <row r="36" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B36" s="5">
-        <f ca="1">IFERROR(OFFSET(B36,-1,0,1,1)+1,"")</f>
+        <f t="shared" ca="1" si="1"/>
         <v>32</v>
       </c>
       <c r="C36" s="6" t="s">
@@ -1840,7 +1864,7 @@
         <v>0.69</v>
       </c>
       <c r="H36" s="26" t="str">
-        <f>IF(G36-J36=0,"",ROUND(G36-J36,2)*100&amp;"% Better")</f>
+        <f t="shared" si="4"/>
         <v>11% Better</v>
       </c>
       <c r="J36" s="24">
@@ -1849,7 +1873,7 @@
     </row>
     <row r="37" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B37" s="5">
-        <f ca="1">IFERROR(OFFSET(B37,-1,0,1,1)+1,"")</f>
+        <f t="shared" ca="1" si="1"/>
         <v>33</v>
       </c>
       <c r="C37" s="6" t="s">
@@ -1868,7 +1892,7 @@
         <v>0.35</v>
       </c>
       <c r="H37" s="26" t="str">
-        <f>IF(G37-J37=0,"",ROUND(G37-J37,2)*100&amp;"% Better")</f>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="J37" s="24">
@@ -1877,7 +1901,7 @@
     </row>
     <row r="38" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B38" s="5">
-        <f ca="1">IFERROR(OFFSET(B38,-1,0,1,1)+1,"")</f>
+        <f t="shared" ca="1" si="1"/>
         <v>34</v>
       </c>
       <c r="C38" s="6" t="s">
@@ -1896,7 +1920,7 @@
         <v>0.18</v>
       </c>
       <c r="H38" s="26" t="str">
-        <f>IF(G38-J38=0,"",ROUND(G38-J38,2)*100&amp;"% Better")</f>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="J38" s="24">
@@ -1905,7 +1929,7 @@
     </row>
     <row r="39" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B39" s="5">
-        <f ca="1">IFERROR(OFFSET(B39,-1,0,1,1)+1,"")</f>
+        <f t="shared" ca="1" si="1"/>
         <v>35</v>
       </c>
       <c r="C39" s="6" t="s">
@@ -1924,7 +1948,7 @@
         <v>0.21</v>
       </c>
       <c r="H39" s="26" t="str">
-        <f>IF(G39-J39=0,"",ROUND(G39-J39,2)*100&amp;"% Better")</f>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="J39" s="24">
@@ -1933,7 +1957,7 @@
     </row>
     <row r="40" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B40" s="5">
-        <f ca="1">IFERROR(OFFSET(B40,-1,0,1,1)+1,"")</f>
+        <f t="shared" ca="1" si="1"/>
         <v>36</v>
       </c>
       <c r="C40" s="6" t="s">
@@ -1952,7 +1976,7 @@
         <v>0.06</v>
       </c>
       <c r="H40" s="26" t="str">
-        <f>IF(G40-J40=0,"",ROUND(G40-J40,2)*100&amp;"% Better")</f>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="J40" s="24">
@@ -1980,7 +2004,7 @@
         <v>0.11</v>
       </c>
       <c r="H41" s="26" t="str">
-        <f t="shared" ref="H41" si="3">IF(G41-J41=0,"",ROUND(G41-J41,2)*100&amp;"% Better")</f>
+        <f t="shared" ref="H41" si="5">IF(G41-J41=0,"",ROUND(G41-J41,2)*100&amp;"% Better")</f>
         <v/>
       </c>
       <c r="J41" s="24">
@@ -2120,7 +2144,7 @@
         <v>0.16</v>
       </c>
       <c r="H46" s="26" t="str">
-        <f t="shared" ref="H46:H51" si="4">IF(G46-J46=0,"",ROUND(G46-J46,2)*100&amp;"% Better")</f>
+        <f t="shared" ref="H46:H51" si="6">IF(G46-J46=0,"",ROUND(G46-J46,2)*100&amp;"% Better")</f>
         <v>16% Better</v>
       </c>
       <c r="J46" s="24">
@@ -2148,7 +2172,7 @@
         <v>0.04</v>
       </c>
       <c r="H47" s="26" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>4% Better</v>
       </c>
       <c r="J47" s="24">
@@ -2176,7 +2200,7 @@
         <v>0.5</v>
       </c>
       <c r="H48" s="26" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>50% Better</v>
       </c>
       <c r="J48" s="24">
@@ -2204,7 +2228,7 @@
         <v>0</v>
       </c>
       <c r="H49" s="26" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="J49" s="24">
@@ -2232,7 +2256,7 @@
         <v>0.24</v>
       </c>
       <c r="H50" s="26" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>24% Better</v>
       </c>
       <c r="J50" s="24">
@@ -2241,7 +2265,7 @@
     </row>
     <row r="51" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B51" s="5">
-        <f ca="1">IFERROR(OFFSET(B51,-1,0,1,1)+1,"")</f>
+        <f t="shared" ref="B51:B56" ca="1" si="7">IFERROR(OFFSET(B51,-1,0,1,1)+1,"")</f>
         <v>47</v>
       </c>
       <c r="C51" s="6" t="s">
@@ -2260,7 +2284,7 @@
         <v>0.35</v>
       </c>
       <c r="H51" s="26" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="J51" s="24">
@@ -2269,7 +2293,7 @@
     </row>
     <row r="52" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B52" s="5">
-        <f ca="1">IFERROR(OFFSET(B52,-1,0,1,1)+1,"")</f>
+        <f t="shared" ca="1" si="7"/>
         <v>48</v>
       </c>
       <c r="C52" s="6" t="s">
@@ -2297,7 +2321,7 @@
     </row>
     <row r="53" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B53" s="5">
-        <f ca="1">IFERROR(OFFSET(B53,-1,0,1,1)+1,"")</f>
+        <f t="shared" ca="1" si="7"/>
         <v>49</v>
       </c>
       <c r="C53" s="6" t="s">
@@ -2325,7 +2349,7 @@
     </row>
     <row r="54" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B54" s="5">
-        <f ca="1">IFERROR(OFFSET(B54,-1,0,1,1)+1,"")</f>
+        <f t="shared" ca="1" si="7"/>
         <v>50</v>
       </c>
       <c r="C54" s="6" t="s">
@@ -2353,7 +2377,7 @@
     </row>
     <row r="55" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B55" s="5">
-        <f ca="1">IFERROR(OFFSET(B55,-1,0,1,1)+1,"")</f>
+        <f t="shared" ca="1" si="7"/>
         <v>51</v>
       </c>
       <c r="C55" s="6" t="s">
@@ -2381,7 +2405,7 @@
     </row>
     <row r="56" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B56" s="5">
-        <f ca="1">IFERROR(OFFSET(B56,-1,0,1,1)+1,"")</f>
+        <f t="shared" ca="1" si="7"/>
         <v>52</v>
       </c>
       <c r="C56" s="6" t="s">
@@ -2428,7 +2452,7 @@
         <v>0.32</v>
       </c>
       <c r="H57" s="26" t="str">
-        <f t="shared" ref="H57:H70" si="5">IF(G57-J57=0,"",ROUND(G57-J57,2)*100&amp;"% Better")</f>
+        <f t="shared" ref="H57:H70" si="8">IF(G57-J57=0,"",ROUND(G57-J57,2)*100&amp;"% Better")</f>
         <v/>
       </c>
       <c r="J57" s="24">
@@ -2456,7 +2480,7 @@
         <v>0.93</v>
       </c>
       <c r="H58" s="26" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="J58" s="24">
@@ -2484,7 +2508,7 @@
         <v>0.43</v>
       </c>
       <c r="H59" s="26" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="J59" s="24">
@@ -2512,7 +2536,7 @@
         <v>0.43</v>
       </c>
       <c r="H60" s="26" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="J60" s="24">
@@ -2540,7 +2564,7 @@
         <v>0.35</v>
       </c>
       <c r="H61" s="26" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="J61" s="24">
@@ -2568,7 +2592,7 @@
         <v>0.4</v>
       </c>
       <c r="H62" s="26" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="J62" s="24">
@@ -2596,7 +2620,7 @@
         <v>0.31</v>
       </c>
       <c r="H63" s="26" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="J63" s="24">
@@ -2624,7 +2648,7 @@
         <v>0.24</v>
       </c>
       <c r="H64" s="26" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="J64" s="24">
@@ -2652,7 +2676,7 @@
         <v>0.38</v>
       </c>
       <c r="H65" s="26" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="J65" s="24">
@@ -2680,7 +2704,7 @@
         <v>0.39</v>
       </c>
       <c r="H66" s="26" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="J66" s="24">
@@ -2708,7 +2732,7 @@
         <v>0.45</v>
       </c>
       <c r="H67" s="26" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="J67" s="24">
@@ -2736,7 +2760,7 @@
         <v>0.09</v>
       </c>
       <c r="H68" s="26" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="J68" s="24">
@@ -2764,7 +2788,7 @@
         <v>0.31</v>
       </c>
       <c r="H69" s="26" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="J69" s="24">
@@ -2792,7 +2816,7 @@
         <v>0.27</v>
       </c>
       <c r="H70" s="26" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="J70" s="24">
@@ -2810,16 +2834,16 @@
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
-  <dimension ref="B2:I18"/>
+  <dimension ref="B2:I22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="2.33203125" customWidth="1"/>
-    <col min="3" max="3" width="61.21875" customWidth="1"/>
+    <col min="3" max="3" width="83.21875" customWidth="1"/>
     <col min="4" max="4" width="19.6640625" customWidth="1"/>
     <col min="5" max="5" width="20.33203125" customWidth="1"/>
     <col min="6" max="6" width="15.109375" customWidth="1"/>
@@ -2846,7 +2870,7 @@
         <v>2</v>
       </c>
       <c r="G3" s="29" t="s">
-        <v>100</v>
+        <v>137</v>
       </c>
     </row>
     <row r="4" spans="2:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -2928,7 +2952,7 @@
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B8" s="16">
-        <f t="shared" ref="B5:B8" ca="1" si="0">IFERROR(OFFSET(B8,-1,0,1,1)+1,"")</f>
+        <f t="shared" ref="B8" ca="1" si="0">IFERROR(OFFSET(B8,-1,0,1,1)+1,"")</f>
         <v>4</v>
       </c>
       <c r="C8" s="17" t="s">
@@ -2947,7 +2971,7 @@
     </row>
     <row r="9" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B9" s="16">
-        <f ca="1">IFERROR(OFFSET(B9,-1,0,1,1)+1,"")</f>
+        <f t="shared" ref="B9:B22" ca="1" si="1">IFERROR(OFFSET(B9,-1,0,1,1)+1,"")</f>
         <v>5</v>
       </c>
       <c r="C9" s="17" t="s">
@@ -2967,7 +2991,7 @@
     </row>
     <row r="10" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B10" s="16">
-        <f ca="1">IFERROR(OFFSET(B10,-1,0,1,1)+1,"")</f>
+        <f t="shared" ca="1" si="1"/>
         <v>6</v>
       </c>
       <c r="C10" s="17" t="s">
@@ -2987,7 +3011,7 @@
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B11" s="16">
-        <f ca="1">IFERROR(OFFSET(B11,-1,0,1,1)+1,"")</f>
+        <f t="shared" ca="1" si="1"/>
         <v>7</v>
       </c>
       <c r="C11" s="17" t="s">
@@ -3007,7 +3031,7 @@
     </row>
     <row r="12" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B12" s="16">
-        <f ca="1">IFERROR(OFFSET(B12,-1,0,1,1)+1,"")</f>
+        <f t="shared" ca="1" si="1"/>
         <v>8</v>
       </c>
       <c r="C12" s="17" t="s">
@@ -3027,7 +3051,7 @@
     </row>
     <row r="13" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B13" s="16">
-        <f ca="1">IFERROR(OFFSET(B13,-1,0,1,1)+1,"")</f>
+        <f t="shared" ca="1" si="1"/>
         <v>9</v>
       </c>
       <c r="C13" s="17" t="s">
@@ -3047,7 +3071,7 @@
     </row>
     <row r="14" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B14" s="16">
-        <f ca="1">IFERROR(OFFSET(B14,-1,0,1,1)+1,"")</f>
+        <f t="shared" ca="1" si="1"/>
         <v>10</v>
       </c>
       <c r="C14" s="17" t="s">
@@ -3067,7 +3091,7 @@
     </row>
     <row r="15" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B15" s="16">
-        <f ca="1">IFERROR(OFFSET(B15,-1,0,1,1)+1,"")</f>
+        <f t="shared" ca="1" si="1"/>
         <v>11</v>
       </c>
       <c r="C15" s="17" t="s">
@@ -3086,7 +3110,7 @@
     </row>
     <row r="16" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B16" s="16">
-        <f ca="1">IFERROR(OFFSET(B16,-1,0,1,1)+1,"")</f>
+        <f t="shared" ca="1" si="1"/>
         <v>12</v>
       </c>
       <c r="C16" s="17" t="s">
@@ -3105,7 +3129,7 @@
     </row>
     <row r="17" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B17" s="16">
-        <f ca="1">IFERROR(OFFSET(B17,-1,0,1,1)+1,"")</f>
+        <f t="shared" ca="1" si="1"/>
         <v>13</v>
       </c>
       <c r="C17" s="17" t="s">
@@ -3125,7 +3149,7 @@
     </row>
     <row r="18" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B18" s="16">
-        <f ca="1">IFERROR(OFFSET(B18,-1,0,1,1)+1,"")</f>
+        <f t="shared" ca="1" si="1"/>
         <v>14</v>
       </c>
       <c r="C18" s="17" t="s">
@@ -3142,6 +3166,82 @@
       </c>
       <c r="G18" s="23"/>
       <c r="I18" s="24"/>
+    </row>
+    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B19" s="16">
+        <f t="shared" ca="1" si="1"/>
+        <v>15</v>
+      </c>
+      <c r="C19" s="17" t="s">
+        <v>135</v>
+      </c>
+      <c r="D19" s="18" t="s">
+        <v>118</v>
+      </c>
+      <c r="E19" s="19" t="s">
+        <v>136</v>
+      </c>
+      <c r="F19" s="20">
+        <v>2024</v>
+      </c>
+      <c r="G19" s="23"/>
+    </row>
+    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B20" s="16">
+        <f t="shared" ca="1" si="1"/>
+        <v>16</v>
+      </c>
+      <c r="C20" s="17" t="s">
+        <v>138</v>
+      </c>
+      <c r="D20" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="E20" s="19" t="s">
+        <v>139</v>
+      </c>
+      <c r="F20" s="20">
+        <v>2024</v>
+      </c>
+      <c r="G20" s="23"/>
+    </row>
+    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B21" s="16">
+        <f t="shared" ca="1" si="1"/>
+        <v>17</v>
+      </c>
+      <c r="C21" s="17" t="s">
+        <v>140</v>
+      </c>
+      <c r="D21" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="E21" s="19" t="s">
+        <v>141</v>
+      </c>
+      <c r="F21" s="20">
+        <v>2024</v>
+      </c>
+      <c r="G21" s="23"/>
+    </row>
+    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B22" s="16">
+        <f t="shared" ca="1" si="1"/>
+        <v>18</v>
+      </c>
+      <c r="C22" s="17" t="s">
+        <v>142</v>
+      </c>
+      <c r="D22" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="E22" s="19" t="s">
+        <v>137</v>
+      </c>
+      <c r="F22" s="20">
+        <v>2024</v>
+      </c>
+      <c r="G22" s="23"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>